<commit_message>
add class 2 files
</commit_message>
<xml_diff>
--- a/JSC370 Schedule - Draft.xlsx
+++ b/JSC370 Schedule - Draft.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathantaback/Dropbox (Personal)/Docs/jsc370/jsc370.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286C04D0-CF09-6649-95A1-1FD27D072D5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AD66B4-A546-C045-8969-EBF3DA0E6462}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27640" yWindow="10420" windowWidth="20280" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21400" yWindow="6260" windowWidth="26520" windowHeight="20460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JSC370-schedule" sheetId="1" r:id="rId1"/>
-    <sheet name="eval" sheetId="2" r:id="rId2"/>
+    <sheet name="TA - Schedule" sheetId="3" r:id="rId2"/>
+    <sheet name="eval" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Z_B47C07D5_D070_42AA_8B1F_83A81D587F90_.wvu.FilterData" localSheetId="0" hidden="1">'JSC370-schedule'!$A$1:$C$27</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -271,6 +272,24 @@
   <si>
     <t>End of course reflection/survey</t>
   </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>JC</t>
+  </si>
+  <si>
+    <t>JC + MM</t>
+  </si>
+  <si>
+    <t>TA conducting lab</t>
+  </si>
+  <si>
+    <t>provide feedback on assignment plan</t>
+  </si>
+  <si>
+    <t>MM grade presentations + provide pres feedback, JC grade presentations</t>
+  </si>
 </sst>
 </file>
 
@@ -279,7 +298,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="ddd&quot;, &quot;mmm&quot; &quot;d&quot;, &quot;yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -306,6 +325,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -348,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -371,6 +396,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,7 +618,7 @@
   <dimension ref="A1:D1008"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3894,10 +3920,447 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5BC17D1-1D1F-584B-A0E7-12B7E50C4240}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="63.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16">
+      <c r="A2" s="4">
+        <v>43837</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="16">
+      <c r="A3" s="4">
+        <v>43839</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="16">
+      <c r="A4" s="6">
+        <v>43844</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16">
+      <c r="A5" s="6">
+        <v>43846</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="16">
+      <c r="A6" s="6">
+        <v>43851</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16">
+      <c r="A7" s="6">
+        <v>43853</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="16">
+      <c r="A8" s="6">
+        <v>43858</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16">
+      <c r="A9" s="6">
+        <v>43860</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16">
+      <c r="A10" s="6">
+        <v>43865</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16">
+      <c r="A11" s="6">
+        <v>43867</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="16">
+      <c r="A12" s="6">
+        <v>43872</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16">
+      <c r="A13" s="6">
+        <v>43874</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16">
+      <c r="A14" s="7">
+        <v>43879</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="16">
+      <c r="A15" s="7">
+        <v>43881</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="16">
+      <c r="A16" s="6">
+        <v>43886</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16">
+      <c r="A17" s="6">
+        <v>43888</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="16">
+      <c r="A18" s="6">
+        <v>43893</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16">
+      <c r="A19" s="6">
+        <v>43895</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16">
+      <c r="A20" s="6">
+        <v>43900</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16">
+      <c r="A21" s="6">
+        <v>43902</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" ht="16">
+      <c r="A22" s="4">
+        <v>43907</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16">
+      <c r="A23" s="11">
+        <v>43909</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16">
+      <c r="A24" s="14">
+        <v>43914</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16">
+      <c r="A25" s="14">
+        <v>43916</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="16">
+      <c r="A26" s="14">
+        <v>43921</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16">
+      <c r="A27" s="14">
+        <v>43923</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE925ED-6A1D-B344-9FCF-21F4E841C72D}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>